<commit_message>
Second commit on  3rd
</commit_message>
<xml_diff>
--- a/Project/src/test/resources/Test Data.xlsx
+++ b/Project/src/test/resources/Test Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\febat\eclipse-workspace\Project\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\febat\git\7r-Mart-Supermarket\Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559132FB-0DBF-4E82-92C3-4C2B19EE52E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9FF78E-0F28-44CB-995B-5500E51BED6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="9984" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3294" yWindow="3294" windowWidth="17280" windowHeight="9984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Feba</t>
+  </si>
+  <si>
+    <t>admin2345</t>
+  </si>
+  <si>
+    <t>admin5678</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -455,6 +461,14 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -519,10 +533,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5A7EB3-380B-4242-8CAD-09E4886BF8DA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -531,28 +545,22 @@
     <col min="2" max="2" width="62.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -566,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAADEED-05C5-4123-8B0C-E647D5CD3FF2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>